<commit_message>
ref: Validation in .xlsx file
</commit_message>
<xml_diff>
--- a/pyengineer/examples/excel/structure_011.xlsx
+++ b/pyengineer/examples/excel/structure_011.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\PyEngineer\pyengineer\examples\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FF681A-D4C9-43D3-ABF2-607127ECA6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138E7798-03AB-407A-9A9D-E0FFE7B79170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{17B9D78E-9B11-469E-9BF6-00D2F9C8B7DE}"/>
   </bookViews>
@@ -20,7 +20,8 @@
     <sheet name="Supports" sheetId="5" r:id="rId5"/>
     <sheet name="Node Loads" sheetId="6" r:id="rId6"/>
     <sheet name="Bar Point Loads" sheetId="7" r:id="rId7"/>
-    <sheet name="Bar Distributed Loads" sheetId="8" r:id="rId8"/>
+    <sheet name="Bar Distributed Loads" sheetId="10" r:id="rId8"/>
+    <sheet name="Data" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
   <si>
     <t>E</t>
   </si>
@@ -51,9 +52,6 @@
     <t>G</t>
   </si>
   <si>
-    <t>ni</t>
-  </si>
-  <si>
     <t>rho</t>
   </si>
   <si>
@@ -238,6 +236,9 @@
   </si>
   <si>
     <t>Fy End</t>
+  </si>
+  <si>
+    <t>nu</t>
   </si>
 </sst>
 </file>
@@ -295,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -307,12 +308,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -651,8 +646,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2827D6D6-99B8-4E1C-AFE0-EC4F81C51153}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
+        <v>200000000000</v>
+      </c>
+      <c r="C2" s="3">
+        <v>76923080000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>7850</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="7">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Nome do Material" prompt="Insira um nome único para cada material." sqref="A1" xr:uid="{D3E51FD3-6CBB-4AF2-A4AE-6DF61E1F0425}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Elasticidade Longitudinal" prompt="Módulo de elasticidade longitudinal." sqref="B1" xr:uid="{17786DE4-A08C-479C-9B5F-ABFB6D43E36A}">
+      <formula1>"EXATO(A1;E)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Elasticidade Transvesal" prompt="Módulo de elasticidade transversal." sqref="C1" xr:uid="{42D45CA5-7CB7-4390-B0F3-D93CBA9E6EA5}">
+      <formula1>"EXATO(A1;G)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Peso Específico" prompt="Peso específico." sqref="E1" xr:uid="{B49F478F-93A1-4160-BA53-C7A5FB9C90F4}">
+      <formula1>"EXATO(A1;rho)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Coeficiente de Poisson" prompt="Coeficiente de Poisson." sqref="D1" xr:uid="{51127C8C-B328-42E7-A06C-5E8E65565BEF}">
+      <formula1>"EXATO(A1;nu)"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número maior que zero._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="C2:E2 B2" xr:uid="{9053EFE6-7AF9-4F20-8A68-F5B7C6074AD4}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um texto._x000a_- Certifíque-se de que não seja um número." sqref="A2" xr:uid="{D001422F-FF4E-46D6-B7A0-BE5127264DA9}">
+      <formula1>ISTEXT(A2)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82A31C1-1787-4B27-88FB-E70EF65F68D6}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -662,88 +746,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3">
-        <v>200000000000</v>
-      </c>
-      <c r="C2" s="3">
-        <v>76923080000</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="E2" s="1">
-        <v>7850</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="4"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82A31C1-1787-4B27-88FB-E70EF65F68D6}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="5" width="8.7265625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="B2" s="3">
         <v>1.6299999999999999E-3</v>
@@ -759,6 +779,29 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="7">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Nome da Seção" prompt="Insira um nome único para cada seção." sqref="A1" xr:uid="{536E1B3A-B725-4EAF-8C17-E33AF7DF1960}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Área" prompt="Área." sqref="B1" xr:uid="{8DDC20F0-05D8-4E5B-9C73-F16A85709B26}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Inércia em X" prompt="Inércia em torno de eixo &quot;x&quot; da seção. Também chamada de inércia polar e representada por &quot;It&quot;." sqref="C1" xr:uid="{5C0D953F-1C37-4B9A-B470-8593F67E71D0}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Inércia em Y" prompt="Inércia em torno de eixo &quot;y&quot; da seção. " sqref="D1" xr:uid="{D44B2E78-3900-400D-995F-6647B258B24A}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Inércia em Z" prompt="Inércia em torno de eixo &quot;z&quot; da seção. " sqref="E1" xr:uid="{8160E394-D8FC-4EFA-9633-150FFAF5174A}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número maior que zero._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="B2:E2" xr:uid="{F6C87C4A-6FBF-4618-AFD6-19A04EA167C7}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um texto._x000a_- Certifíque-se de que não seja um número." sqref="A2" xr:uid="{2A42D855-5982-4E6A-9E72-9C360E31FEAE}">
+      <formula1>ISTEXT(A2)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -768,32 +811,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8664EE-4B7A-42F3-BD1B-3377E942A26C}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="4" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -807,7 +851,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -821,7 +865,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>5</v>
@@ -835,7 +879,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
@@ -852,6 +896,26 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Nome do Nó" prompt="Insira um nome único para cada nó._x000a__x000a_NOTAS:_x000a_- Cuidado para não sobrepor nós._x000a_- Nós muito próximos ( &lt; 0,1 m) pondem gerar resultados equivocados." sqref="A1" xr:uid="{4E700B3B-1614-4713-BB14-B81B6D484558}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Posição em X" prompt="Posição do nó no eixo &quot;x&quot; global." sqref="B1" xr:uid="{359CDC6B-6EC6-4471-BCD3-8F7E5FBB7D3C}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Posiçaõ em Y" prompt="Posição do nó no eixo &quot;y&quot; global." sqref="C1" xr:uid="{8AA87B7D-C5BF-42F2-8698-4BF0277E1984}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Posição em Z" prompt="Posição do nó no eixo &quot;z&quot; global." sqref="D1" xr:uid="{46B2C3CC-03D1-44B8-911F-777F5E579F7E}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="C2:D5 B3:B5 B2" xr:uid="{9465AC62-7BE0-47DB-93D1-D5B4ADFDA056}">
+      <formula1>ISNUMBER(B2)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um texto._x000a_- Certifíque-se de que não seja um número." sqref="A2:A5" xr:uid="{5D017D99-03BC-4415-B9D6-030C77844AD5}">
+      <formula1>ISTEXT(A2)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -861,7 +925,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -869,104 +933,158 @@
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="11.08984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.08984375" style="1" customWidth="1"/>
-    <col min="4" max="6" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="1"/>
     <col min="7" max="7" width="11.54296875" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1">
         <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1">
         <v>30</v>
       </c>
-      <c r="G4" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="9">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Nome da Barra" prompt="Insira um nome único para cada barra." sqref="A1" xr:uid="{402B903C-B963-4011-8EC6-F1A988287ECE}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Nó Inicial" prompt="NOTAS:_x000a_-A orientação dos eixo locais e, conseguentemente, a posição das cargas na barra, são influenciadas de acordo com qual nó é o primeiro._x000a_- O eixo &quot;x&quot; local vai do nó inicial para o nó final e o eixo &quot;z&quot; tenta apontar para o &quot;z&quot; global._x000a_" sqref="B1" xr:uid="{BE4ACE1A-6684-4225-94C7-91BF1E770B8E}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Nó Final" prompt="NOTAS:_x000a_-A orientação dos eixo locais e, conseguentemente, a posição das cargas na barra, são influenciadas de acordo com qual nó é o primeiro._x000a_- O eixo &quot;x&quot; local vai do nó inicial para o nó final e o eixo &quot;z&quot; tenta apontar para o &quot;z&quot; global." sqref="C1" xr:uid="{D62CD3B1-E310-438F-B69A-C102AD6AAB26}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Material" prompt="Insira o nome dado ao material na aba &quot;Materials&quot;." sqref="D1" xr:uid="{2D8877CB-C3C6-498A-B802-0EA38664FB0D}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Seção" prompt="Insira o nome dado a seção na aba &quot;Sections&quot;." sqref="E1" xr:uid="{FB288B62-6ED1-497C-86B6-4686E23B82C0}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Rotação (°)" prompt="Rotação, em graus, da barra em torno do eixo &quot;x&quot; lcal._x000a_Isso influencia os eixos locais da barra" sqref="F1" xr:uid="{FDB6DCA5-7CF5-45AA-AFC8-8060406A6E7E}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Liberações" prompt="Siga o padrão:_x000a_&quot;D&quot; (Maiúsculo) para deslocamento e &quot;R&quot; para rotação_x000a_&quot;x&quot;, &quot;y&quot; e &quot;z&quot; (Minúsculo) para indicar a direção_x000a_&quot;i&quot; ou &quot;j&quot; para indicar nó inicial ou final respectivamente._x000a_&quot;;&quot; para separar._x000a_Ex.: Dxi; Dzi; Ryi; Ryj" sqref="G1" xr:uid="{B3D86EDB-65C3-4D5B-8A8D-DA8ED532988A}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="F2:F4" xr:uid="{62AB4244-273E-4B4D-8AFF-7A3A986FF70B}">
+      <formula1>ISNUMBER(F2)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um texto._x000a_- Certifíque-se de que não seja um número." sqref="A2:A4" xr:uid="{84A50396-4B7F-4640-ACD7-0CE0F4899FAB}">
+      <formula1>ISTEXT(A2)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Material Inexistente" error="Insira um material cadastrado na aba &quot;Materials&quot;." xr:uid="{D5E6120D-E702-43A1-B786-EB6FC002B28A}">
+          <x14:formula1>
+            <xm:f>OFFSET(Materials!$A$2,0,0,COUNTA(Materials!$A:$A)-1,1)</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Nó Inexistente" error="Insira um nó cadastrado na aba &quot;Nodes&quot;." xr:uid="{B5B97569-ED30-48E6-84D6-76DB77EE5B1E}">
+          <x14:formula1>
+            <xm:f>OFFSET(Nodes!$A$2,0,0,COUNTA(Nodes!$A:$A)-1,1)</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Seção Inxistente" error="Insira uma seção cadastrada na aba &quot;Sections&quot;" xr:uid="{54048A7C-393F-4933-AB0D-D1FF5BD6921C}">
+          <x14:formula1>
+            <xm:f>OFFSET(Sections!$A$2,0,0,COUNTA(Sections!$A:$A)-1,1)</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -974,95 +1092,136 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B57BFD-4F1D-437A-B710-E4A8DC974E0E}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="8" width="8.7265625" style="1"/>
+    <col min="1" max="2" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="8">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Nó" prompt="Nó em que será inserido o suporte._x000a_Cada nó pode ter um único suporte._x000a_suporte é o mesmo que apoio." sqref="A1" xr:uid="{F28EC543-DBDD-4766-802C-F6CC4EAA40CA}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Deslocamento em X" prompt="- &quot;True&quot; para fixar_x000a_- &quot;False&quot; para liberar_x000a_- Um número para apoio mola (N/m)." sqref="B1" xr:uid="{4A71928C-342C-4D84-81F5-06F998162E9C}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Deslocamento em Y" prompt="- &quot;True&quot; para fixar_x000a_- &quot;False&quot; para liberar_x000a_- Um número para apoio mola (N/m)." sqref="C1" xr:uid="{B7AC0618-E9FA-4E1A-B916-9066FC37F156}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Deslocamento em Z" prompt="- &quot;True&quot; para fixar_x000a_- &quot;False&quot; para liberar_x000a_- Um número para apoio mola (N/m)." sqref="D1" xr:uid="{5CA2CD9F-5622-4D81-BF14-5F1102C1E2C4}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Rotação em X" prompt="- &quot;True&quot; para fixar_x000a_- &quot;False&quot; para liberar_x000a_- Um número para apoio mola (N/m)." sqref="E1" xr:uid="{57B8275C-A7E2-4261-B0F2-A133D4B78D63}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Rotação em Y" prompt="- &quot;True&quot; para fixar_x000a_- &quot;False&quot; para liberar_x000a_- Um número para apoio mola (N/m)." sqref="F1" xr:uid="{52F5F4D6-D05F-48B5-88AC-DDF176289EA5}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Rotação em Z" prompt="- &quot;True&quot; para fixar_x000a_- &quot;False&quot; para liberar_x000a_- Um número para apoio mola (N/m)." sqref="G1" xr:uid="{DF537B87-D742-4AD8-BBAD-A7EE1170FA3B}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira:_x000a_- &quot;True&quot;: Para fixar_x000a_- &quot;False&quot;: Para liberar_x000a_- Um número: Para apoio mola." sqref="B2:G3" xr:uid="{09CF8805-F6B3-41BE-99A3-11488589CA16}">
+      <formula1>OR(EXACT(B2,"True"),EXACT(B2,"False"),ISNUMBER(B2))</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Nó Inexistente" error="Insira um nó cadastrado na aba &quot;Nodes&quot;." xr:uid="{E6E61560-17A3-447E-8223-1FFDA4F799D5}">
+          <x14:formula1>
+            <xm:f>OFFSET(Nodes!$A$2,0,0,COUNTA(Nodes!$A:$A)-1,1)</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2EA52E0-332D-4A5B-93D8-29009A3F2596}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:H2"/>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1072,36 +1231,36 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3">
         <v>1000</v>
@@ -1122,8 +1281,60 @@
         <v>6000</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
   </sheetData>
+  <dataValidations count="10">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Nome da Carga" prompt="Insira um nome único para cada carga." sqref="A1" xr:uid="{DF22BC29-5C53-4202-BA6D-29952DF1A094}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Nó" prompt="Nó onde a carga será inserida." sqref="B1" xr:uid="{A1AED69A-2001-494D-AEF7-F320C609B48C}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Força em X (N)" prompt="Força na direção do eixo &quot;x&quot;" sqref="C1" xr:uid="{71EDC53E-66DA-4DB3-9495-2383C014FA44}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Força em Y (N)" prompt="Força na direção do eixo &quot;y&quot;" sqref="D1" xr:uid="{3534CFE4-30CE-494E-8B29-8A734202C4CC}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Força em Z (N)" prompt="Força na direção do eixo &quot;z&quot;" sqref="E1" xr:uid="{7D52A555-8C72-46C9-9FF5-CA335DA8C014}">
+      <formula1>"EXATO(A1;Name)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Momento em X (N*m)" prompt="Momento na direção do eixo &quot;x&quot;" sqref="F1" xr:uid="{31A408CD-5E57-4F94-BCD6-BF744173A203}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Momento em Y (N*m)" prompt="Momento na direção do eixo &quot;y&quot;" sqref="G1" xr:uid="{D5DF2176-89DF-4130-B685-BE81A4DF1991}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Momento em Z (N*m)" prompt="Momento na direção do eixo &quot;z&quot;" sqref="H1" xr:uid="{C037DA2C-BA11-4828-AD2B-6DF1969B3899}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um texto._x000a_- Certifíque-se de que não seja um número." sqref="A2" xr:uid="{86797EB4-D6E4-46E9-B845-D6147D273EF3}">
+      <formula1>ISTEXT(A2)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="C2:H3" xr:uid="{DC9FB40D-2B32-4DF7-B9EB-067D03BCFA77}">
+      <formula1>ISNUMBER(C2)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Nó Inexistente" error="Insira um nó cadastrado na aba &quot;Nodes&quot;." xr:uid="{0351FF88-A04C-4287-9C83-07C3D1A728F1}">
+          <x14:formula1>
+            <xm:f>OFFSET(Nodes!$A$2,0,0,COUNTA(Nodes!$A:$A)-1,1)</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1131,8 +1342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D8020E7-CF35-4686-B894-429A41C784D5}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1142,45 +1353,45 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1205,16 +1416,75 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="13">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Nome da Carga" prompt="Insira um nome único para a carga pontual." sqref="A1" xr:uid="{0B296BB2-5AC5-46B0-8F1E-07720FBD16A2}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Barra" prompt="Barra em que a carga será inserida." sqref="B1" xr:uid="{1D47ED91-8585-4E0A-8590-278E8548068B}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Sitema" prompt="Sistema usado para a orientação da carga. Pode ser:_x000a_&quot;Local&quot; - Segue o sistema da barra. Se a barra estiver rotacionada a carga também rotacionará._x000a_&quot;Global&quot; - Segue o sistema global e não é influenciado pela rotação da barra." sqref="C1" xr:uid="{353B5148-6ABF-448D-942C-C18094BA257A}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Posição (m)" prompt="Posição onde a carga será inserida." sqref="D1" xr:uid="{2232ABB8-FD6B-4FBB-B73F-05830A64E397}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Força em X (N)" prompt="Força na direção do eixo &quot;x&quot;" sqref="E1" xr:uid="{8A8E88E5-CBAF-4567-8E22-1DFF81BF6B7A}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Força em Y (N)" prompt="Força na direção do eixo &quot;y&quot;" sqref="F1" xr:uid="{1B8AC11B-DDF1-4022-A121-3D3B9B933CC4}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Força em Z (N)" prompt="Força na direção do eixo &quot;z&quot;" sqref="G1" xr:uid="{5883135B-4E94-447A-968C-7B47C9017E95}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Momento em X (N*m)" prompt="Momento na direção do eixo &quot;x&quot;" sqref="H1" xr:uid="{A8820D6D-6C8C-44C3-98D6-E826EAA95759}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Momento em Y (N*m)" prompt="Momento na direção do eixo &quot;y&quot;" sqref="I1" xr:uid="{53D35E6B-D31B-4BD7-B05F-FC593A972FB0}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Momento em Z (N*m)" prompt="Momento na direção do eixo &quot;z&quot;" sqref="J1" xr:uid="{BAB381DB-4925-45F1-9068-D0F1D900F679}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um texto._x000a_- Certifíque-se de que não seja um número." sqref="A2" xr:uid="{B245C836-DFF8-4945-9187-D83BC327A026}">
+      <formula1>ISTEXT(A2)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número &gt;= 0._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="D2" xr:uid="{A2D7F8B0-DAF8-4C33-BAF9-FE6768977322}">
+      <formula1>AND(D2&gt;=0,ISNUMBER(D2))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="F2:J2 E2" xr:uid="{99A116DD-A993-4FEF-A31F-6503FB7783CE}">
+      <formula1>ISNUMBER(E2)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Barra Inexistente" error="Insira uma barra cadastrada na aba &quot;Bars&quot;." xr:uid="{351C5E99-835C-4AEA-B610-2801B1D7711D}">
+          <x14:formula1>
+            <xm:f>OFFSET(Bars!$A$2,0,0,COUNTA(Bars!$A:$A)-1,1)</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sistema Inválido" error="O sistema deve ser &quot;Local&quot; ou &quot;Global&quot; escrito dessa mesma forma com atenção para primeira letra ser maiúscula." xr:uid="{E55A6936-9AE4-44CF-9D10-00761F79BD75}">
+          <x14:formula1>
+            <xm:f>Data!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DBF098B-B9D6-4AB8-9B5B-F26A8830A5D8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74033608-E1CC-4E7B-B66A-375D48222978}">
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1224,74 +1494,74 @@
     <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="8.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="8.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D2" s="1">
         <v>0.5</v>
@@ -1299,44 +1569,150 @@
       <c r="E2" s="1">
         <v>3.5</v>
       </c>
-      <c r="F2" s="6">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6">
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
         <v>-1000</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="3">
         <v>-3000</v>
       </c>
-      <c r="L2" s="6">
-        <v>0</v>
-      </c>
-      <c r="M2" s="6">
-        <v>0</v>
-      </c>
-      <c r="N2" s="6">
-        <v>0</v>
-      </c>
-      <c r="O2" s="6">
-        <v>0</v>
-      </c>
-      <c r="P2" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>0</v>
-      </c>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>0</v>
+      </c>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+    </row>
+  </sheetData>
+  <dataValidations count="21">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Posição Final" prompt="Onde a carga termina._x000a_Onde a carga começa._x000a_- Deve ser um valor &gt; 0 e &lt;= ao comprimento da barra." sqref="E1" xr:uid="{99A14947-9E28-4D4A-BA65-373BC4D3C68E}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Sistema" prompt="Sistema usado para a orientação da carga. Pode ser:_x000a_&quot;Local&quot; - Segue o sistema da barra. Se a barra estiver rotacionada a carga também rotacionará._x000a_&quot;Global&quot; - Segue o sistema global e não é influenciado pela rotação da barra." sqref="C1" xr:uid="{040E8C0B-0184-44C9-8014-A30AC38427C8}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Barra" prompt="Barra onde a carga será inserida." sqref="B1" xr:uid="{04AC7146-341B-4691-8355-BCACF0A8D2E7}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Nome da Carga" prompt="Insira um nome único para cada carga distribuída." sqref="A1" xr:uid="{A831F7AB-0CAF-4F8D-9D01-2993BF9A34F2}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Posição Incial" prompt="Onde a carga começa._x000a_- Deve ser um valor &gt;= 0 e &lt; que o comprimento da barra." sqref="D1" xr:uid="{2016B21A-8D6B-46A5-AFD1-93E6831E5D46}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Força em X Inicial (N)" prompt="Força na direção do eixo &quot;x&quot; no começo da barra" sqref="F1" xr:uid="{BD8721F2-B857-47AB-A8BB-959B8D116226}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Força em X Final (N)" prompt="Força na direção do eixo &quot;x&quot; no final da Barra" sqref="G1" xr:uid="{BD162997-C8A5-4E88-9DEE-1A0FE28B7013}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Força em Y Inicial (N)" prompt="Força na direção do eixo &quot;y&quot; no início da barra." sqref="H1" xr:uid="{BE09F801-8436-48D0-BFF7-E77DB2925BC1}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Força em Z Inicial (N)" prompt="Força na direção do eixo &quot;z&quot; no começo da barra" sqref="J1" xr:uid="{F0027B0A-F09B-4552-A6AB-9601E446508B}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Momento em X Inicial (N*m)" prompt="Momento na direção do eixo &quot;x&quot; no início da barra." sqref="L1" xr:uid="{1184BBA7-3782-48A3-8E01-768A9344E5CE}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Momento em Y Inicial (N*m)" prompt="Momento na direção do eixo &quot;y&quot; no início da barra." sqref="N1" xr:uid="{4FF22455-C1B2-4883-BE3D-0985DE1F66C9}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Momento em Z Inicial (N*m)" prompt="Momento na direção do eixo &quot;z&quot; no início da barra." sqref="P1" xr:uid="{C39129F8-D553-4A8B-96A5-2F5A4E4B9707}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Força em Y Final (N)" prompt="Força na direção do eixo &quot;y&quot; no final da Barra" sqref="I1" xr:uid="{DD4F33C2-09FF-46F9-A7B0-294A4E16971E}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Força em Z Final (N)" prompt="Força na direção do eixo &quot;z&quot; no final da Barra" sqref="K1" xr:uid="{F7F34D7F-EA76-41FB-8E21-0BFC95F9D283}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Momento em X Final (N*m)" prompt="Momento na direção do eixo &quot;x&quot; no final da barra." sqref="M1" xr:uid="{D899F006-88EE-4062-A04C-9BD8EDF7A641}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Momento em Y Final (N*m)" prompt="Momento na direção do eixo &quot;y&quot; no final da barra." sqref="O1" xr:uid="{07B97F12-3C75-4EA7-BB5A-807831A13498}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Momento em Z Final (N*m)" prompt="Momento na direção do eixo &quot;z&quot; no final da barra." sqref="Q1" xr:uid="{B7FC6F06-3F68-48D8-99B5-C44B3E6CA6D4}">
+      <formula1>"bloqueada"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um texto._x000a_- Certifíque-se de que não seja um número." sqref="A2" xr:uid="{82EC8606-F12C-4DFE-AD5B-35F10C607376}">
+      <formula1>ISTEXT(A2)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número&gt;= 0._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="D2" xr:uid="{C949EF88-D82D-4A0B-AD21-9964D0ECF74A}">
+      <formula1>AND(D2&gt;=0,ISNUMBER(D2))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número &gt; 0._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="E2" xr:uid="{02820B3E-1F21-493D-AB01-9CDD983C27DD}">
+      <formula1>AND(E2&gt;0,ISNUMBER(E2))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="F2:Q2" xr:uid="{90240017-4CFE-4872-BBD0-B8570585AC9A}">
+      <formula1>ISNUMBER(F2)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sistema Inválido" error="O sistema deve ser &quot;Local&quot; ou &quot;Global&quot; escrito dessa mesma forma com atenção para primeira letra ser maiúscula." xr:uid="{35EEF2DC-61B6-472F-A295-294F220B1953}">
+          <x14:formula1>
+            <xm:f>Data!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Barra Inexistente" error="Insira uma barra cadastrada na aba &quot;Bars&quot;." xr:uid="{18DD2507-D3D0-4E5B-A5ED-932D11D7A9F9}">
+          <x14:formula1>
+            <xm:f>OFFSET(Bars!$A$2,0,0,COUNTA(Bars!$A:$A)-1,1)</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F1D8D4-836C-4925-B21F-6D90AE64BBB0}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>